<commit_message>
10 29 2016 yyy
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/payaccount-testdata.xlsx
+++ b/src/main/resources/testdata/payaccount-testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="5355" windowWidth="25920" windowHeight="12645" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="1755" yWindow="5355" windowWidth="25920" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="pay_order" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,6 +354,10 @@
   </si>
   <si>
     <t>OC201607181150225991</t>
+  </si>
+  <si>
+    <t>2016-07-18 11:47:31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -805,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -823,7 +827,14 @@
     <col min="10" max="10" width="30.375" customWidth="1"/>
     <col min="11" max="11" width="25.5" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="16" max="16" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27" customWidth="1"/>
+    <col min="17" max="17" width="22.125" customWidth="1"/>
+    <col min="18" max="18" width="20.125" customWidth="1"/>
+    <col min="19" max="19" width="21.125" customWidth="1"/>
+    <col min="20" max="20" width="25.25" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="13.75" customWidth="1"/>
+    <col min="23" max="23" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -967,7 +978,12 @@
       <c r="R2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="2"/>
+      <c r="S2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" t="s">
+        <v>42</v>
+      </c>
       <c r="U2">
         <v>0</v>
       </c>
@@ -1044,7 +1060,12 @@
       <c r="R3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S3" s="2"/>
+      <c r="S3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
       <c r="U3">
         <v>0</v>
       </c>
@@ -1198,14 +1219,20 @@
       <c r="O5">
         <v>1</v>
       </c>
-      <c r="P5" s="3">
-        <v>42568.493958333333</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>42569.493310185186</v>
-      </c>
-      <c r="R5" s="3">
-        <v>42569.493958333333</v>
+      <c r="P5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T5" t="s">
+        <v>42</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -1864,7 +1891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>